<commit_message>
Rename LLM to SSA-LLM and add hosting variants
Changes:
- Renamed "LLM" service to "SSA-LLM"
- Added hosting variants for supported services:
  - Full Support (In-Region)
  - Full Support (Cross-Region)
  - Limited Support (In-Region)
  - Limited Support (Cross-Region)
  - Not Supported
- Updated conditional formatting with distinct colors for each variant
- Updated product dashboard formulas to handle new status format

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Product Language Matrix/Smart_Availability_Matrix.xlsx
+++ b/Product Language Matrix/Smart_Availability_Matrix.xlsx
@@ -111,7 +111,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="00FFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00375623"/>
+          <bgColor rgb="00375623"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="00FFFFFF"/>
@@ -120,6 +131,17 @@
         <patternFill patternType="solid">
           <fgColor rgb="0070AD47"/>
           <bgColor rgb="0070AD47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="00FFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00BF8F00"/>
+          <bgColor rgb="00BF8F00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -560,7 +582,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E2">
@@ -612,7 +634,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E4">
@@ -638,7 +660,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E5">
@@ -664,7 +686,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E6">
@@ -690,7 +712,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E7">
@@ -716,7 +738,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E8">
@@ -742,7 +764,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E9">
@@ -768,7 +790,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E10">
@@ -794,7 +816,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E11">
@@ -820,7 +842,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E12">
@@ -846,7 +868,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E13">
@@ -872,7 +894,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E14">
@@ -898,7 +920,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E15">
@@ -924,7 +946,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E16">
@@ -950,7 +972,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E17">
@@ -976,7 +998,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E18">
@@ -1054,7 +1076,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E21">
@@ -1080,7 +1102,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E22">
@@ -1132,7 +1154,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E24">
@@ -1184,7 +1206,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E26">
@@ -1236,7 +1258,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E28">
@@ -1262,7 +1284,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E29">
@@ -1288,7 +1310,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E30">
@@ -1314,7 +1336,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E31">
@@ -1340,7 +1362,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E32">
@@ -1366,7 +1388,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E33">
@@ -1392,7 +1414,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E34">
@@ -1418,7 +1440,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E35">
@@ -1444,7 +1466,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E36">
@@ -1470,7 +1492,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E37">
@@ -1496,7 +1518,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E38">
@@ -1522,7 +1544,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E39">
@@ -1548,7 +1570,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E40">
@@ -1574,7 +1596,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E41">
@@ -1600,7 +1622,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E42">
@@ -1626,7 +1648,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E43">
@@ -1652,7 +1674,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E44">
@@ -1704,7 +1726,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E46">
@@ -1730,7 +1752,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E47">
@@ -1756,7 +1778,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E48">
@@ -1782,7 +1804,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E49">
@@ -1808,7 +1830,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E50">
@@ -1834,7 +1856,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E51">
@@ -1860,7 +1882,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E52">
@@ -1886,7 +1908,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E53">
@@ -1912,7 +1934,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E54">
@@ -1938,7 +1960,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E55">
@@ -1990,7 +2012,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E57">
@@ -2016,7 +2038,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E58">
@@ -2042,7 +2064,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E59">
@@ -2068,7 +2090,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E60">
@@ -2094,7 +2116,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E61">
@@ -2146,7 +2168,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E63">
@@ -2172,7 +2194,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E64">
@@ -2188,7 +2210,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2198,7 +2220,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E65">
@@ -2214,7 +2236,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2240,7 +2262,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2250,7 +2272,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E67">
@@ -2266,7 +2288,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2276,7 +2298,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E68">
@@ -2292,7 +2314,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2302,7 +2324,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E69">
@@ -2318,7 +2340,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2328,7 +2350,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E70">
@@ -2344,7 +2366,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2354,7 +2376,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E71">
@@ -2380,7 +2402,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E72">
@@ -2406,7 +2428,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E73">
@@ -2432,7 +2454,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E74">
@@ -2458,7 +2480,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E75">
@@ -2484,7 +2506,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E76">
@@ -2510,7 +2532,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E77">
@@ -2536,7 +2558,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E78">
@@ -2562,7 +2584,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E79">
@@ -2588,7 +2610,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E80">
@@ -2614,7 +2636,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E81">
@@ -2640,7 +2662,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E82">
@@ -2666,7 +2688,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E83">
@@ -2692,7 +2714,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E84">
@@ -2718,7 +2740,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E85">
@@ -2770,7 +2792,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E87">
@@ -2796,7 +2818,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E88">
@@ -2822,7 +2844,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E89">
@@ -2848,7 +2870,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E90">
@@ -2900,7 +2922,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E92">
@@ -2926,7 +2948,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E93">
@@ -2952,7 +2974,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E94">
@@ -2978,7 +3000,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E95">
@@ -3004,7 +3026,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E96">
@@ -3030,7 +3052,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E97">
@@ -3056,7 +3078,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E98">
@@ -3082,7 +3104,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E99">
@@ -3108,7 +3130,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E100">
@@ -3134,7 +3156,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E101">
@@ -3160,7 +3182,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E102">
@@ -3186,7 +3208,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E103">
@@ -3212,7 +3234,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E104">
@@ -3238,7 +3260,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E105">
@@ -3264,7 +3286,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E106">
@@ -3290,7 +3312,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E107">
@@ -3316,7 +3338,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E108">
@@ -3342,7 +3364,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E109">
@@ -3368,7 +3390,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E110">
@@ -3394,7 +3416,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E111">
@@ -3446,7 +3468,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E113">
@@ -3472,7 +3494,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E114">
@@ -3498,7 +3520,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E115">
@@ -3524,7 +3546,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E116">
@@ -3550,7 +3572,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E117">
@@ -3576,7 +3598,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E118">
@@ -3602,7 +3624,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E119">
@@ -3628,7 +3650,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E120">
@@ -3654,7 +3676,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E121">
@@ -3680,7 +3702,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E122">
@@ -3706,7 +3728,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E123">
@@ -3732,7 +3754,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E124">
@@ -3758,7 +3780,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E125">
@@ -3784,7 +3806,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E126">
@@ -3810,7 +3832,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E127">
@@ -3862,7 +3884,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E129">
@@ -3888,7 +3910,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E130">
@@ -3914,7 +3936,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E131">
@@ -3940,7 +3962,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E132">
@@ -3966,7 +3988,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E133">
@@ -3992,7 +4014,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E134">
@@ -4018,7 +4040,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E135">
@@ -4044,7 +4066,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E136">
@@ -4070,7 +4092,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E137">
@@ -4096,7 +4118,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E138">
@@ -4122,7 +4144,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E139">
@@ -4148,7 +4170,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E140">
@@ -4174,7 +4196,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E141">
@@ -4190,7 +4212,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -4200,7 +4222,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E142">
@@ -4216,7 +4238,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -4226,7 +4248,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E143">
@@ -4242,7 +4264,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -4268,7 +4290,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -4278,7 +4300,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E145">
@@ -4294,7 +4316,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -4320,7 +4342,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -4330,7 +4352,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E147">
@@ -4346,7 +4368,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -4408,7 +4430,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E150">
@@ -4434,7 +4456,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E151">
@@ -4460,7 +4482,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E152">
@@ -4486,7 +4508,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E153">
@@ -4564,7 +4586,7 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E156">
@@ -4590,7 +4612,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E157">
@@ -4616,7 +4638,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E158">
@@ -4642,7 +4664,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E159">
@@ -4694,7 +4716,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E161">
@@ -4720,7 +4742,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E162">
@@ -4746,7 +4768,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E163">
@@ -4798,7 +4820,7 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E165">
@@ -4824,7 +4846,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E166">
@@ -4850,7 +4872,7 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E167">
@@ -4928,7 +4950,7 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E170">
@@ -4954,7 +4976,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E171">
@@ -4980,7 +5002,7 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E172">
@@ -5006,7 +5028,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E173">
@@ -5032,7 +5054,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E174">
@@ -5058,7 +5080,7 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E175">
@@ -5084,7 +5106,7 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E176">
@@ -5110,7 +5132,7 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E177">
@@ -5136,7 +5158,7 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E178">
@@ -5162,7 +5184,7 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E179">
@@ -5188,7 +5210,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E180">
@@ -5214,7 +5236,7 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E181">
@@ -5240,7 +5262,7 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E182">
@@ -5266,7 +5288,7 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E183">
@@ -5292,7 +5314,7 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E184">
@@ -5318,7 +5340,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E185">
@@ -5344,7 +5366,7 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E186">
@@ -5370,7 +5392,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E187">
@@ -5396,7 +5418,7 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E188">
@@ -5422,7 +5444,7 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E189">
@@ -5448,7 +5470,7 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E190">
@@ -5500,7 +5522,7 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E192">
@@ -5526,7 +5548,7 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E193">
@@ -5552,7 +5574,7 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E194">
@@ -5578,7 +5600,7 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E195">
@@ -5604,7 +5626,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E196">
@@ -5630,7 +5652,7 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E197">
@@ -5656,7 +5678,7 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E198">
@@ -5682,7 +5704,7 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E199">
@@ -5708,7 +5730,7 @@
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E200">
@@ -5734,7 +5756,7 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E201">
@@ -5760,7 +5782,7 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E202">
@@ -5786,7 +5808,7 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E203">
@@ -5812,7 +5834,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E204">
@@ -5864,7 +5886,7 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E206">
@@ -5890,7 +5912,7 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E207">
@@ -5916,7 +5938,7 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E208">
@@ -5968,7 +5990,7 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E210">
@@ -5994,7 +6016,7 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E211">
@@ -6020,7 +6042,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E212">
@@ -6046,7 +6068,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E213">
@@ -6072,7 +6094,7 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E214">
@@ -6098,7 +6120,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E215">
@@ -6124,7 +6146,7 @@
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E216">
@@ -6150,7 +6172,7 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E217">
@@ -6176,7 +6198,7 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E218">
@@ -6192,7 +6214,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -6202,7 +6224,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E219">
@@ -6218,7 +6240,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
@@ -6228,7 +6250,7 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E220">
@@ -6244,7 +6266,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
@@ -6254,7 +6276,7 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E221">
@@ -6270,7 +6292,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -6296,7 +6318,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
@@ -6306,7 +6328,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E223">
@@ -6322,7 +6344,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -6332,7 +6354,7 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E224">
@@ -6348,7 +6370,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
@@ -6358,7 +6380,7 @@
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E225">
@@ -6384,7 +6406,7 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E226">
@@ -6410,7 +6432,7 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E227">
@@ -6436,7 +6458,7 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E228">
@@ -6462,7 +6484,7 @@
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E229">
@@ -6488,7 +6510,7 @@
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E230">
@@ -6540,7 +6562,7 @@
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E232">
@@ -6566,7 +6588,7 @@
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E233">
@@ -6592,7 +6614,7 @@
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E234">
@@ -6618,7 +6640,7 @@
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E235">
@@ -6644,7 +6666,7 @@
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E236">
@@ -6670,7 +6692,7 @@
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E237">
@@ -6696,7 +6718,7 @@
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E238">
@@ -6722,7 +6744,7 @@
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E239">
@@ -6748,7 +6770,7 @@
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E240">
@@ -6774,7 +6796,7 @@
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E241">
@@ -6800,7 +6822,7 @@
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E242">
@@ -6826,7 +6848,7 @@
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E243">
@@ -6852,7 +6874,7 @@
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E244">
@@ -6904,7 +6926,7 @@
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E246">
@@ -6930,7 +6952,7 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E247">
@@ -6956,7 +6978,7 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E248">
@@ -6982,7 +7004,7 @@
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E249">
@@ -7008,7 +7030,7 @@
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E250">
@@ -7034,7 +7056,7 @@
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E251">
@@ -7060,7 +7082,7 @@
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E252">
@@ -7086,7 +7108,7 @@
       </c>
       <c r="D253" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E253">
@@ -7112,7 +7134,7 @@
       </c>
       <c r="D254" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E254">
@@ -7138,7 +7160,7 @@
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E255">
@@ -7164,7 +7186,7 @@
       </c>
       <c r="D256" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E256">
@@ -7190,7 +7212,7 @@
       </c>
       <c r="D257" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E257">
@@ -7216,7 +7238,7 @@
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E258">
@@ -7242,7 +7264,7 @@
       </c>
       <c r="D259" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E259">
@@ -7268,7 +7290,7 @@
       </c>
       <c r="D260" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E260">
@@ -7294,7 +7316,7 @@
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E261">
@@ -7320,7 +7342,7 @@
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E262">
@@ -7346,7 +7368,7 @@
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E263">
@@ -7372,7 +7394,7 @@
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E264">
@@ -7398,7 +7420,7 @@
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E265">
@@ -7424,7 +7446,7 @@
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E266">
@@ -7450,7 +7472,7 @@
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E267">
@@ -7476,7 +7498,7 @@
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E268">
@@ -7528,7 +7550,7 @@
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E270">
@@ -7554,7 +7576,7 @@
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E271">
@@ -7580,7 +7602,7 @@
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E272">
@@ -7632,7 +7654,7 @@
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E274">
@@ -7658,7 +7680,7 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E275">
@@ -7684,7 +7706,7 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E276">
@@ -7710,7 +7732,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E277">
@@ -7736,7 +7758,7 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E278">
@@ -7762,7 +7784,7 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E279">
@@ -7788,7 +7810,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E280">
@@ -7840,7 +7862,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E282">
@@ -7866,7 +7888,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E283">
@@ -7892,7 +7914,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E284">
@@ -7944,7 +7966,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E286">
@@ -7970,7 +7992,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E287">
@@ -7996,7 +8018,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E288">
@@ -8022,7 +8044,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E289">
@@ -8074,7 +8096,7 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E291">
@@ -8100,7 +8122,7 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E292">
@@ -8126,7 +8148,7 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E293">
@@ -8152,7 +8174,7 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E294">
@@ -8178,7 +8200,7 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E295">
@@ -8194,7 +8216,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -8204,7 +8226,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E296">
@@ -8220,7 +8242,7 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -8230,7 +8252,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E297">
@@ -8246,7 +8268,7 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -8256,7 +8278,7 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E298">
@@ -8272,7 +8294,7 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -8282,7 +8304,7 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E299">
@@ -8298,7 +8320,7 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -8308,7 +8330,7 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E300">
@@ -8324,7 +8346,7 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -8334,7 +8356,7 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E301">
@@ -8350,7 +8372,7 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -8360,7 +8382,7 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E302">
@@ -8386,7 +8408,7 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E303">
@@ -8412,7 +8434,7 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E304">
@@ -8438,7 +8460,7 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E305">
@@ -8464,7 +8486,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E306">
@@ -8490,7 +8512,7 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E307">
@@ -8516,7 +8538,7 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E308">
@@ -8542,7 +8564,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E309">
@@ -8568,7 +8590,7 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E310">
@@ -8594,7 +8616,7 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E311">
@@ -8620,7 +8642,7 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E312">
@@ -8646,7 +8668,7 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E313">
@@ -8672,7 +8694,7 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E314">
@@ -8724,7 +8746,7 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E316">
@@ -8750,7 +8772,7 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E317">
@@ -8776,7 +8798,7 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E318">
@@ -8802,7 +8824,7 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E319">
@@ -8828,7 +8850,7 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E320">
@@ -8854,7 +8876,7 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E321">
@@ -8880,7 +8902,7 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E322">
@@ -8906,7 +8928,7 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E323">
@@ -8958,7 +8980,7 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E325">
@@ -8984,7 +9006,7 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E326">
@@ -9010,7 +9032,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E327">
@@ -9036,7 +9058,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E328">
@@ -9062,7 +9084,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E329">
@@ -9114,7 +9136,7 @@
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E331">
@@ -9140,7 +9162,7 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E332">
@@ -9166,7 +9188,7 @@
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E333">
@@ -9192,7 +9214,7 @@
       </c>
       <c r="D334" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E334">
@@ -9218,7 +9240,7 @@
       </c>
       <c r="D335" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E335">
@@ -9244,7 +9266,7 @@
       </c>
       <c r="D336" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E336">
@@ -9270,7 +9292,7 @@
       </c>
       <c r="D337" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E337">
@@ -9296,7 +9318,7 @@
       </c>
       <c r="D338" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E338">
@@ -9322,7 +9344,7 @@
       </c>
       <c r="D339" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E339">
@@ -9348,7 +9370,7 @@
       </c>
       <c r="D340" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E340">
@@ -9374,7 +9396,7 @@
       </c>
       <c r="D341" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E341">
@@ -9400,7 +9422,7 @@
       </c>
       <c r="D342" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E342">
@@ -9426,7 +9448,7 @@
       </c>
       <c r="D343" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E343">
@@ -9452,7 +9474,7 @@
       </c>
       <c r="D344" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E344">
@@ -9478,7 +9500,7 @@
       </c>
       <c r="D345" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E345">
@@ -9504,7 +9526,7 @@
       </c>
       <c r="D346" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E346">
@@ -9530,7 +9552,7 @@
       </c>
       <c r="D347" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E347">
@@ -9556,7 +9578,7 @@
       </c>
       <c r="D348" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E348">
@@ -9582,7 +9604,7 @@
       </c>
       <c r="D349" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E349">
@@ -9608,7 +9630,7 @@
       </c>
       <c r="D350" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E350">
@@ -9634,7 +9656,7 @@
       </c>
       <c r="D351" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E351">
@@ -9660,7 +9682,7 @@
       </c>
       <c r="D352" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E352">
@@ -9712,7 +9734,7 @@
       </c>
       <c r="D354" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E354">
@@ -9738,7 +9760,7 @@
       </c>
       <c r="D355" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E355">
@@ -9764,7 +9786,7 @@
       </c>
       <c r="D356" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E356">
@@ -9816,7 +9838,7 @@
       </c>
       <c r="D358" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E358">
@@ -9868,7 +9890,7 @@
       </c>
       <c r="D360" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E360">
@@ -9894,7 +9916,7 @@
       </c>
       <c r="D361" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E361">
@@ -9920,7 +9942,7 @@
       </c>
       <c r="D362" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E362">
@@ -9946,7 +9968,7 @@
       </c>
       <c r="D363" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E363">
@@ -9972,7 +9994,7 @@
       </c>
       <c r="D364" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E364">
@@ -9998,7 +10020,7 @@
       </c>
       <c r="D365" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E365">
@@ -10024,7 +10046,7 @@
       </c>
       <c r="D366" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E366">
@@ -10050,7 +10072,7 @@
       </c>
       <c r="D367" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E367">
@@ -10076,7 +10098,7 @@
       </c>
       <c r="D368" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E368">
@@ -10102,7 +10124,7 @@
       </c>
       <c r="D369" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E369">
@@ -10128,7 +10150,7 @@
       </c>
       <c r="D370" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E370">
@@ -10180,7 +10202,7 @@
       </c>
       <c r="D372" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E372">
@@ -10196,7 +10218,7 @@
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C373" t="inlineStr">
@@ -10206,7 +10228,7 @@
       </c>
       <c r="D373" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E373">
@@ -10222,7 +10244,7 @@
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C374" t="inlineStr">
@@ -10232,7 +10254,7 @@
       </c>
       <c r="D374" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E374">
@@ -10248,7 +10270,7 @@
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C375" t="inlineStr">
@@ -10258,7 +10280,7 @@
       </c>
       <c r="D375" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E375">
@@ -10274,7 +10296,7 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C376" t="inlineStr">
@@ -10284,7 +10306,7 @@
       </c>
       <c r="D376" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E376">
@@ -10300,7 +10322,7 @@
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C377" t="inlineStr">
@@ -10310,7 +10332,7 @@
       </c>
       <c r="D377" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E377">
@@ -10326,7 +10348,7 @@
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C378" t="inlineStr">
@@ -10336,7 +10358,7 @@
       </c>
       <c r="D378" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E378">
@@ -10352,7 +10374,7 @@
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="C379" t="inlineStr">
@@ -10362,7 +10384,7 @@
       </c>
       <c r="D379" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E379">
@@ -10388,7 +10410,7 @@
       </c>
       <c r="D380" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E380">
@@ -10414,7 +10436,7 @@
       </c>
       <c r="D381" t="inlineStr">
         <is>
-          <t>Limited Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E381">
@@ -10440,7 +10462,7 @@
       </c>
       <c r="D382" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E382">
@@ -10466,7 +10488,7 @@
       </c>
       <c r="D383" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E383">
@@ -10492,7 +10514,7 @@
       </c>
       <c r="D384" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E384">
@@ -10518,7 +10540,7 @@
       </c>
       <c r="D385" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E385">
@@ -10544,7 +10566,7 @@
       </c>
       <c r="D386" t="inlineStr">
         <is>
-          <t>Full Support</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E386">
@@ -10657,7 +10679,7 @@
       </c>
       <c r="K7" s="5" t="inlineStr">
         <is>
-          <t>LLM</t>
+          <t>SSA-LLM</t>
         </is>
       </c>
       <c r="L7" s="5" t="inlineStr">
@@ -11025,13 +11047,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B8:L14">
-    <cfRule type="containsText" priority="1" operator="containsText" dxfId="0" text="Full Support">
-      <formula>NOT(ISERROR(SEARCH("Full Support", B8:L14)))</formula>
+    <cfRule type="containsText" priority="1" operator="containsText" dxfId="0" text="Full Support (In-Region)">
+      <formula>NOT(ISERROR(SEARCH("Full Support (In-Region)", B8:L14)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="2" operator="containsText" dxfId="1" text="Limited Support">
-      <formula>NOT(ISERROR(SEARCH("Limited Support", B8:L14)))</formula>
+    <cfRule type="containsText" priority="2" operator="containsText" dxfId="1" text="Full Support (Cross-Region)">
+      <formula>NOT(ISERROR(SEARCH("Full Support (Cross-Region)", B8:L14)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="3" operator="containsText" dxfId="2" text="Not Supported">
+    <cfRule type="containsText" priority="3" operator="containsText" dxfId="2" text="Limited Support (In-Region)">
+      <formula>NOT(ISERROR(SEARCH("Limited Support (In-Region)", B8:L14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="4" operator="containsText" dxfId="3" text="Limited Support (Cross-Region)">
+      <formula>NOT(ISERROR(SEARCH("Limited Support (Cross-Region)", B8:L14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="5" operator="containsText" dxfId="4" text="Not Supported">
       <formula>NOT(ISERROR(SEARCH("Not Supported", B8:L14)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11123,19 +11151,19 @@
         </is>
       </c>
       <c r="B8" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|LLM|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|LLM|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
       <c r="C8" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
       <c r="D8" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
       <c r="E8" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
     </row>
@@ -11146,19 +11174,19 @@
         </is>
       </c>
       <c r="B9" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|LLM|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|LLM|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
       <c r="C9" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
       <c r="D9" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
       <c r="E9" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
     </row>
@@ -11169,19 +11197,19 @@
         </is>
       </c>
       <c r="B10" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|LLM|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|LLM|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
       <c r="C10" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
       <c r="D10" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
       <c r="E10" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
     </row>
@@ -11192,19 +11220,19 @@
         </is>
       </c>
       <c r="B11" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|LLM|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|LLM|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
       <c r="C11" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
       <c r="D11" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
       <c r="E11" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
     </row>
@@ -11215,19 +11243,19 @@
         </is>
       </c>
       <c r="B12" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|LLM|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|LLM|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
       <c r="C12" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
       <c r="D12" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
       <c r="E12" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
     </row>
@@ -11238,19 +11266,19 @@
         </is>
       </c>
       <c r="B13" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|LLM|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|LLM|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
       <c r="C13" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
       <c r="D13" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
       <c r="E13" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
     </row>
@@ -11261,31 +11289,37 @@
         </is>
       </c>
       <c r="B14" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|LLM|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|LLM|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
       <c r="C14" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
       <c r="D14" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
       <c r="E14" s="9">
-        <f>IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported"), "Not Supported", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Support"), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
         <v/>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B8:E14">
-    <cfRule type="containsText" priority="1" operator="containsText" dxfId="0" text="Full Support">
-      <formula>NOT(ISERROR(SEARCH("Full Support", B8:E14)))</formula>
+    <cfRule type="containsText" priority="1" operator="containsText" dxfId="0" text="Full Support (In-Region)">
+      <formula>NOT(ISERROR(SEARCH("Full Support (In-Region)", B8:E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="2" operator="containsText" dxfId="1" text="Limited Support">
-      <formula>NOT(ISERROR(SEARCH("Limited Support", B8:E14)))</formula>
+    <cfRule type="containsText" priority="2" operator="containsText" dxfId="1" text="Full Support (Cross-Region)">
+      <formula>NOT(ISERROR(SEARCH("Full Support (Cross-Region)", B8:E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="3" operator="containsText" dxfId="2" text="Not Supported">
+    <cfRule type="containsText" priority="3" operator="containsText" dxfId="2" text="Limited Support (In-Region)">
+      <formula>NOT(ISERROR(SEARCH("Limited Support (In-Region)", B8:E14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="4" operator="containsText" dxfId="3" text="Limited Support (Cross-Region)">
+      <formula>NOT(ISERROR(SEARCH("Limited Support (Cross-Region)", B8:E14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="5" operator="containsText" dxfId="4" text="Not Supported">
       <formula>NOT(ISERROR(SEARCH("Not Supported", B8:E14)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add hosting variants to Product Dashboard
Product Dashboard now shows hosting type (In-Region/Cross-Region):
- If any dependency is Cross-Region, product shows Cross-Region
- If all dependencies are In-Region, product shows In-Region

Both Service and Product dashboards now display:
- Full Support (In-Region)
- Full Support (Cross-Region)
- Limited Support (In-Region)
- Limited Support (Cross-Region)
- Not Supported

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Product Language Matrix/Smart_Availability_Matrix.xlsx
+++ b/Product Language Matrix/Smart_Availability_Matrix.xlsx
@@ -634,7 +634,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E4">
@@ -686,7 +686,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E6">
@@ -738,7 +738,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E8">
@@ -764,7 +764,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E9">
@@ -816,7 +816,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E11">
@@ -842,7 +842,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E12">
@@ -868,7 +868,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E13">
@@ -894,7 +894,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E14">
@@ -920,7 +920,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E15">
@@ -946,7 +946,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E16">
@@ -998,7 +998,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E18">
@@ -1024,7 +1024,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E19">
@@ -1102,7 +1102,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E22">
@@ -1128,7 +1128,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E23">
@@ -1154,7 +1154,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E24">
@@ -1180,7 +1180,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E25">
@@ -1206,7 +1206,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E26">
@@ -1232,7 +1232,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E27">
@@ -1258,7 +1258,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E28">
@@ -1310,7 +1310,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E30">
@@ -1336,7 +1336,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E31">
@@ -1362,7 +1362,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E32">
@@ -1388,7 +1388,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E33">
@@ -1414,7 +1414,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E34">
@@ -1440,7 +1440,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E35">
@@ -1466,7 +1466,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E36">
@@ -1492,7 +1492,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E37">
@@ -1518,7 +1518,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E38">
@@ -1544,7 +1544,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E39">
@@ -1570,7 +1570,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E40">
@@ -1596,7 +1596,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E41">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E43">
@@ -1674,7 +1674,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E44">
@@ -1700,7 +1700,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E45">
@@ -1726,7 +1726,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E46">
@@ -1752,7 +1752,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E47">
@@ -1778,7 +1778,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E48">
@@ -1804,7 +1804,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E49">
@@ -1830,7 +1830,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E50">
@@ -1856,7 +1856,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E51">
@@ -1882,7 +1882,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E52">
@@ -1908,7 +1908,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E53">
@@ -1934,7 +1934,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E54">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E55">
@@ -1986,7 +1986,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E56">
@@ -2038,7 +2038,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E58">
@@ -2064,7 +2064,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E59">
@@ -2090,7 +2090,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E60">
@@ -2142,7 +2142,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E62">
@@ -2168,7 +2168,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E63">
@@ -2194,7 +2194,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E64">
@@ -2220,7 +2220,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E65">
@@ -2246,7 +2246,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E66">
@@ -2272,7 +2272,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E67">
@@ -2298,7 +2298,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E68">
@@ -2324,7 +2324,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E69">
@@ -2350,7 +2350,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E70">
@@ -2376,7 +2376,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E71">
@@ -2402,7 +2402,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E72">
@@ -2454,7 +2454,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E74">
@@ -2480,7 +2480,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E75">
@@ -2506,7 +2506,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E76">
@@ -2532,7 +2532,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E77">
@@ -2558,7 +2558,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E78">
@@ -2584,7 +2584,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E79">
@@ -2636,7 +2636,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E81">
@@ -2662,7 +2662,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E82">
@@ -2688,7 +2688,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E83">
@@ -2714,7 +2714,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E84">
@@ -2740,7 +2740,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E85">
@@ -2766,7 +2766,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E86">
@@ -2792,7 +2792,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E87">
@@ -2818,7 +2818,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E88">
@@ -2844,7 +2844,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E89">
@@ -2896,7 +2896,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E91">
@@ -2922,7 +2922,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E92">
@@ -2948,7 +2948,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E93">
@@ -2974,7 +2974,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E94">
@@ -3000,7 +3000,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E95">
@@ -3026,7 +3026,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E96">
@@ -3052,7 +3052,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E97">
@@ -3104,7 +3104,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E99">
@@ -3130,7 +3130,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E100">
@@ -3156,7 +3156,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E101">
@@ -3182,7 +3182,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E102">
@@ -3208,7 +3208,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E103">
@@ -3234,7 +3234,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E104">
@@ -3260,7 +3260,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E105">
@@ -3286,7 +3286,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E106">
@@ -3312,7 +3312,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E107">
@@ -3338,7 +3338,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E108">
@@ -3364,7 +3364,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E109">
@@ -3390,7 +3390,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E110">
@@ -3416,7 +3416,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E111">
@@ -3442,7 +3442,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E112">
@@ -3494,7 +3494,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E114">
@@ -3520,7 +3520,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E115">
@@ -3546,7 +3546,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E116">
@@ -3572,7 +3572,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E117">
@@ -3598,7 +3598,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E118">
@@ -3624,7 +3624,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E119">
@@ -3650,7 +3650,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E120">
@@ -3676,7 +3676,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E121">
@@ -3702,7 +3702,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E122">
@@ -3728,7 +3728,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E123">
@@ -3754,7 +3754,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E124">
@@ -3780,7 +3780,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E125">
@@ -3806,7 +3806,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E126">
@@ -3832,7 +3832,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E127">
@@ -3858,7 +3858,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E128">
@@ -3884,7 +3884,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E129">
@@ -3936,7 +3936,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E131">
@@ -3962,7 +3962,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E132">
@@ -3988,7 +3988,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E133">
@@ -4014,7 +4014,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E134">
@@ -4040,7 +4040,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E135">
@@ -4066,7 +4066,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E136">
@@ -4092,7 +4092,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E137">
@@ -4118,7 +4118,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E138">
@@ -4144,7 +4144,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E139">
@@ -4196,7 +4196,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E141">
@@ -4248,7 +4248,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E143">
@@ -4274,7 +4274,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E144">
@@ -4300,7 +4300,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E145">
@@ -4404,7 +4404,7 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E149">
@@ -4430,7 +4430,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E150">
@@ -4456,7 +4456,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E151">
@@ -4482,7 +4482,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E152">
@@ -4508,7 +4508,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E153">
@@ -4560,7 +4560,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E155">
@@ -4586,7 +4586,7 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E156">
@@ -4612,7 +4612,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E157">
@@ -4638,7 +4638,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E158">
@@ -4664,7 +4664,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E159">
@@ -4690,7 +4690,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E160">
@@ -4716,7 +4716,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E161">
@@ -4742,7 +4742,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E162">
@@ -4768,7 +4768,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E163">
@@ -4794,7 +4794,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E164">
@@ -4820,7 +4820,7 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E165">
@@ -4846,7 +4846,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E166">
@@ -4872,7 +4872,7 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E167">
@@ -4898,7 +4898,7 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E168">
@@ -4924,7 +4924,7 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E169">
@@ -4976,7 +4976,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E171">
@@ -5002,7 +5002,7 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E172">
@@ -5028,7 +5028,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E173">
@@ -5054,7 +5054,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E174">
@@ -5080,7 +5080,7 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E175">
@@ -5106,7 +5106,7 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E176">
@@ -5132,7 +5132,7 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E177">
@@ -5158,7 +5158,7 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E178">
@@ -5184,7 +5184,7 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E179">
@@ -5210,7 +5210,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E180">
@@ -5236,7 +5236,7 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E181">
@@ -5262,7 +5262,7 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E182">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E183">
@@ -5314,7 +5314,7 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E184">
@@ -5340,7 +5340,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E185">
@@ -5392,7 +5392,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E187">
@@ -5418,7 +5418,7 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E188">
@@ -5470,7 +5470,7 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E190">
@@ -5496,7 +5496,7 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E191">
@@ -5522,7 +5522,7 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E192">
@@ -5548,7 +5548,7 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E193">
@@ -5574,7 +5574,7 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E194">
@@ -5600,7 +5600,7 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E195">
@@ -5626,7 +5626,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E196">
@@ -5652,7 +5652,7 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E197">
@@ -5678,7 +5678,7 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E198">
@@ -5704,7 +5704,7 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E199">
@@ -5756,7 +5756,7 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E201">
@@ -5782,7 +5782,7 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E202">
@@ -5808,7 +5808,7 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E203">
@@ -5860,7 +5860,7 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E205">
@@ -5886,7 +5886,7 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E206">
@@ -5912,7 +5912,7 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E207">
@@ -5938,7 +5938,7 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E208">
@@ -5990,7 +5990,7 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E210">
@@ -6016,7 +6016,7 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E211">
@@ -6042,7 +6042,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E212">
@@ -6068,7 +6068,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E213">
@@ -6094,7 +6094,7 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E214">
@@ -6120,7 +6120,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E215">
@@ -6146,7 +6146,7 @@
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E216">
@@ -6172,7 +6172,7 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E217">
@@ -6198,7 +6198,7 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E218">
@@ -6224,7 +6224,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E219">
@@ -6276,7 +6276,7 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E221">
@@ -6328,7 +6328,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E223">
@@ -6354,7 +6354,7 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E224">
@@ -6380,7 +6380,7 @@
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E225">
@@ -6432,7 +6432,7 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E227">
@@ -6458,7 +6458,7 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E228">
@@ -6484,7 +6484,7 @@
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E229">
@@ -6510,7 +6510,7 @@
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E230">
@@ -6536,7 +6536,7 @@
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E231">
@@ -6562,7 +6562,7 @@
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E232">
@@ -6588,7 +6588,7 @@
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E233">
@@ -6614,7 +6614,7 @@
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E234">
@@ -6640,7 +6640,7 @@
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E235">
@@ -6692,7 +6692,7 @@
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E237">
@@ -6744,7 +6744,7 @@
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E239">
@@ -6822,7 +6822,7 @@
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E242">
@@ -6848,7 +6848,7 @@
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E243">
@@ -6874,7 +6874,7 @@
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E244">
@@ -6926,7 +6926,7 @@
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E246">
@@ -6952,7 +6952,7 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E247">
@@ -6978,7 +6978,7 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E248">
@@ -7004,7 +7004,7 @@
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E249">
@@ -7030,7 +7030,7 @@
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E250">
@@ -7056,7 +7056,7 @@
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E251">
@@ -7082,7 +7082,7 @@
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E252">
@@ -7134,7 +7134,7 @@
       </c>
       <c r="D254" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E254">
@@ -7160,7 +7160,7 @@
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E255">
@@ -7186,7 +7186,7 @@
       </c>
       <c r="D256" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E256">
@@ -7212,7 +7212,7 @@
       </c>
       <c r="D257" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E257">
@@ -7264,7 +7264,7 @@
       </c>
       <c r="D259" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E259">
@@ -7290,7 +7290,7 @@
       </c>
       <c r="D260" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E260">
@@ -7316,7 +7316,7 @@
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E261">
@@ -7342,7 +7342,7 @@
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E262">
@@ -7368,7 +7368,7 @@
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E263">
@@ -7394,7 +7394,7 @@
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E264">
@@ -7446,7 +7446,7 @@
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E266">
@@ -7498,7 +7498,7 @@
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E268">
@@ -7524,7 +7524,7 @@
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E269">
@@ -7550,7 +7550,7 @@
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E270">
@@ -7576,7 +7576,7 @@
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E271">
@@ -7628,7 +7628,7 @@
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E273">
@@ -7680,7 +7680,7 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E275">
@@ -7706,7 +7706,7 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E276">
@@ -7732,7 +7732,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E277">
@@ -7758,7 +7758,7 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E278">
@@ -7784,7 +7784,7 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E279">
@@ -7810,7 +7810,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E280">
@@ -7836,7 +7836,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E281">
@@ -7888,7 +7888,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E283">
@@ -7914,7 +7914,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E284">
@@ -7940,7 +7940,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E285">
@@ -7966,7 +7966,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E286">
@@ -7992,7 +7992,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E287">
@@ -8018,7 +8018,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E288">
@@ -8044,7 +8044,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E289">
@@ -8070,7 +8070,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E290">
@@ -8096,7 +8096,7 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E291">
@@ -8122,7 +8122,7 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E292">
@@ -8174,7 +8174,7 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E294">
@@ -8200,7 +8200,7 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E295">
@@ -8226,7 +8226,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E296">
@@ -8252,7 +8252,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E297">
@@ -8330,7 +8330,7 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E300">
@@ -8356,7 +8356,7 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E301">
@@ -8382,7 +8382,7 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E302">
@@ -8512,7 +8512,7 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E307">
@@ -8538,7 +8538,7 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E308">
@@ -8564,7 +8564,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E309">
@@ -8616,7 +8616,7 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E311">
@@ -8642,7 +8642,7 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E312">
@@ -8668,7 +8668,7 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E313">
@@ -8694,7 +8694,7 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E314">
@@ -8720,7 +8720,7 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E315">
@@ -8746,7 +8746,7 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E316">
@@ -8798,7 +8798,7 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E318">
@@ -8824,7 +8824,7 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E319">
@@ -8850,7 +8850,7 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E320">
@@ -8876,7 +8876,7 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E321">
@@ -8902,7 +8902,7 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E322">
@@ -8928,7 +8928,7 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E323">
@@ -8954,7 +8954,7 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E324">
@@ -8980,7 +8980,7 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E325">
@@ -9006,7 +9006,7 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E326">
@@ -9032,7 +9032,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E327">
@@ -9058,7 +9058,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E328">
@@ -9084,7 +9084,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E329">
@@ -9110,7 +9110,7 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E330">
@@ -9136,7 +9136,7 @@
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E331">
@@ -9162,7 +9162,7 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E332">
@@ -9188,7 +9188,7 @@
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E333">
@@ -9214,7 +9214,7 @@
       </c>
       <c r="D334" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E334">
@@ -9240,7 +9240,7 @@
       </c>
       <c r="D335" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E335">
@@ -9266,7 +9266,7 @@
       </c>
       <c r="D336" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E336">
@@ -9318,7 +9318,7 @@
       </c>
       <c r="D338" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E338">
@@ -9396,7 +9396,7 @@
       </c>
       <c r="D341" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E341">
@@ -9422,7 +9422,7 @@
       </c>
       <c r="D342" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E342">
@@ -9448,7 +9448,7 @@
       </c>
       <c r="D343" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E343">
@@ -9474,7 +9474,7 @@
       </c>
       <c r="D344" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E344">
@@ -9500,7 +9500,7 @@
       </c>
       <c r="D345" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E345">
@@ -9526,7 +9526,7 @@
       </c>
       <c r="D346" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E346">
@@ -9552,7 +9552,7 @@
       </c>
       <c r="D347" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E347">
@@ -9578,7 +9578,7 @@
       </c>
       <c r="D348" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E348">
@@ -9604,7 +9604,7 @@
       </c>
       <c r="D349" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E349">
@@ -9630,7 +9630,7 @@
       </c>
       <c r="D350" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E350">
@@ -9656,7 +9656,7 @@
       </c>
       <c r="D351" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E351">
@@ -9682,7 +9682,7 @@
       </c>
       <c r="D352" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E352">
@@ -9760,7 +9760,7 @@
       </c>
       <c r="D355" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E355">
@@ -9786,7 +9786,7 @@
       </c>
       <c r="D356" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E356">
@@ -9812,7 +9812,7 @@
       </c>
       <c r="D357" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E357">
@@ -9864,7 +9864,7 @@
       </c>
       <c r="D359" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E359">
@@ -9890,7 +9890,7 @@
       </c>
       <c r="D360" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E360">
@@ -9916,7 +9916,7 @@
       </c>
       <c r="D361" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E361">
@@ -9942,7 +9942,7 @@
       </c>
       <c r="D362" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E362">
@@ -9968,7 +9968,7 @@
       </c>
       <c r="D363" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E363">
@@ -9994,7 +9994,7 @@
       </c>
       <c r="D364" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E364">
@@ -10020,7 +10020,7 @@
       </c>
       <c r="D365" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E365">
@@ -10046,7 +10046,7 @@
       </c>
       <c r="D366" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E366">
@@ -10072,7 +10072,7 @@
       </c>
       <c r="D367" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E367">
@@ -10098,7 +10098,7 @@
       </c>
       <c r="D368" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E368">
@@ -10150,7 +10150,7 @@
       </c>
       <c r="D370" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E370">
@@ -10228,7 +10228,7 @@
       </c>
       <c r="D373" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E373">
@@ -10254,7 +10254,7 @@
       </c>
       <c r="D374" t="inlineStr">
         <is>
-          <t>Full Support (In-Region)</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E374">
@@ -10280,7 +10280,7 @@
       </c>
       <c r="D375" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E375">
@@ -10306,7 +10306,7 @@
       </c>
       <c r="D376" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E376">
@@ -10332,7 +10332,7 @@
       </c>
       <c r="D377" t="inlineStr">
         <is>
-          <t>Limited Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E377">
@@ -10358,7 +10358,7 @@
       </c>
       <c r="D378" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E378">
@@ -10384,7 +10384,7 @@
       </c>
       <c r="D379" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Limited Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E379">
@@ -10436,7 +10436,7 @@
       </c>
       <c r="D381" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E381">
@@ -10462,7 +10462,7 @@
       </c>
       <c r="D382" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E382">
@@ -10488,7 +10488,7 @@
       </c>
       <c r="D383" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Full Support (Cross-Region)</t>
         </is>
       </c>
       <c r="E383">
@@ -10514,7 +10514,7 @@
       </c>
       <c r="D384" t="inlineStr">
         <is>
-          <t>Full Support (Cross-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E384">
@@ -10540,7 +10540,7 @@
       </c>
       <c r="D385" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Support (In-Region)</t>
         </is>
       </c>
       <c r="E385">
@@ -10566,7 +10566,7 @@
       </c>
       <c r="D386" t="inlineStr">
         <is>
-          <t>Limited Support (In-Region)</t>
+          <t>Full Support (In-Region)</t>
         </is>
       </c>
       <c r="E386">
@@ -11151,19 +11151,19 @@
         </is>
       </c>
       <c r="B8" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="C8" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="D8" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="E8" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
     </row>
@@ -11174,19 +11174,19 @@
         </is>
       </c>
       <c r="B9" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="C9" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="D9" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="E9" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
     </row>
@@ -11197,19 +11197,19 @@
         </is>
       </c>
       <c r="B10" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="C10" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="D10" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="E10" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
     </row>
@@ -11220,19 +11220,19 @@
         </is>
       </c>
       <c r="B11" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="C11" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="D11" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="E11" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
     </row>
@@ -11243,19 +11243,19 @@
         </is>
       </c>
       <c r="B12" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="C12" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="D12" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="E12" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
     </row>
@@ -11266,19 +11266,19 @@
         </is>
       </c>
       <c r="B13" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="C13" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="D13" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="E13" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
     </row>
@@ -11289,19 +11289,19 @@
         </is>
       </c>
       <c r="B14" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="C14" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="D14" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="E14" s="9">
-        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))))), "Limited Support", "Full Support"))</f>
+        <f>IF(OR(ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Not Supported", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))))), "Not Supported", IF(OR(ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Limited Support", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))))), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))))), "Limited Support (Cross-Region)", "Limited Support (In-Region)"), IF(OR(ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0)))), ISNUMBER(SEARCH("Cross-Region", INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))))), "Full Support (Cross-Region)", "Full Support (In-Region)")))</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Change Not Supported logic to >50% threshold
Product is now "Not Supported" only if MORE than 50% of its
dependencies are not supported globally.

If ≤50% dependencies are not supported globally, the product
shows "Limited Availability" instead.

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Product Language Matrix/Smart_Availability_Matrix.xlsx
+++ b/Product Language Matrix/Smart_Availability_Matrix.xlsx
@@ -596,7 +596,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E3">
@@ -622,7 +622,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E4">
@@ -648,7 +648,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E5">
@@ -674,7 +674,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E6">
@@ -700,7 +700,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E7">
@@ -726,7 +726,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E8">
@@ -778,7 +778,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E10">
@@ -804,7 +804,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E11">
@@ -830,7 +830,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E12">
@@ -856,7 +856,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E13">
@@ -882,7 +882,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E14">
@@ -986,7 +986,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E18">
@@ -1064,7 +1064,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E21">
@@ -1142,7 +1142,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E24">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E25">
@@ -1194,7 +1194,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E26">
@@ -1220,7 +1220,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E27">
@@ -1246,7 +1246,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E28">
@@ -1272,7 +1272,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E29">
@@ -1298,7 +1298,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E30">
@@ -1324,7 +1324,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E31">
@@ -1350,7 +1350,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E32">
@@ -1402,7 +1402,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E34">
@@ -1428,7 +1428,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E35">
@@ -1454,7 +1454,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E36">
@@ -1480,7 +1480,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E37">
@@ -1506,7 +1506,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E38">
@@ -1532,7 +1532,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E39">
@@ -1636,7 +1636,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E43">
@@ -1662,7 +1662,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E44">
@@ -1714,7 +1714,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E46">
@@ -1740,7 +1740,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E47">
@@ -1792,7 +1792,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E49">
@@ -1818,7 +1818,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E50">
@@ -1870,7 +1870,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E52">
@@ -1922,7 +1922,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E54">
@@ -1974,7 +1974,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E56">
@@ -2000,7 +2000,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E57">
@@ -2026,7 +2026,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E58">
@@ -2052,7 +2052,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E59">
@@ -2104,7 +2104,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E61">
@@ -2182,7 +2182,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E64">
@@ -2208,7 +2208,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E65">
@@ -2234,7 +2234,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E66">
@@ -2312,7 +2312,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E69">
@@ -2338,7 +2338,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E70">
@@ -2364,7 +2364,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E71">
@@ -2416,7 +2416,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E73">
@@ -2494,7 +2494,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E76">
@@ -2520,7 +2520,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E77">
@@ -2572,7 +2572,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E79">
@@ -2598,7 +2598,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E80">
@@ -2650,7 +2650,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E82">
@@ -2676,7 +2676,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E83">
@@ -2702,7 +2702,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E84">
@@ -2728,7 +2728,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E85">
@@ -2754,7 +2754,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E86">
@@ -2780,7 +2780,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E87">
@@ -2858,7 +2858,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E90">
@@ -2884,7 +2884,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E91">
@@ -2910,7 +2910,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E92">
@@ -2962,7 +2962,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E94">
@@ -2988,7 +2988,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E95">
@@ -3014,7 +3014,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E96">
@@ -3040,7 +3040,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E97">
@@ -3144,7 +3144,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E101">
@@ -3248,7 +3248,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E105">
@@ -3326,7 +3326,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E108">
@@ -3352,7 +3352,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E109">
@@ -3378,7 +3378,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E110">
@@ -3404,7 +3404,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E111">
@@ -3456,7 +3456,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E113">
@@ -3534,7 +3534,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E116">
@@ -3586,7 +3586,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E118">
@@ -3638,7 +3638,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E120">
@@ -3664,7 +3664,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E121">
@@ -3716,7 +3716,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E123">
@@ -3742,7 +3742,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E124">
@@ -3768,7 +3768,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E125">
@@ -3794,7 +3794,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E126">
@@ -3820,7 +3820,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E127">
@@ -3872,7 +3872,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E129">
@@ -3898,7 +3898,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E130">
@@ -3924,7 +3924,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E131">
@@ -3950,7 +3950,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E132">
@@ -4002,7 +4002,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E134">
@@ -4054,7 +4054,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E136">
@@ -4106,7 +4106,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E138">
@@ -4158,7 +4158,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E140">
@@ -4184,7 +4184,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E141">
@@ -4236,7 +4236,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E143">
@@ -4262,7 +4262,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E144">
@@ -4340,7 +4340,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E147">
@@ -4418,7 +4418,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E150">
@@ -4470,7 +4470,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E152">
@@ -4522,7 +4522,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E154">
@@ -4548,7 +4548,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E155">
@@ -4626,7 +4626,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E158">
@@ -4652,7 +4652,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E159">
@@ -4678,7 +4678,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E160">
@@ -4730,7 +4730,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E162">
@@ -4834,7 +4834,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E166">
@@ -4860,7 +4860,7 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E167">
@@ -4886,7 +4886,7 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E168">
@@ -4964,7 +4964,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E171">
@@ -4990,7 +4990,7 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E172">
@@ -5016,7 +5016,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E173">
@@ -5042,7 +5042,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E174">
@@ -5068,7 +5068,7 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E175">
@@ -5094,7 +5094,7 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E176">
@@ -5120,7 +5120,7 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E177">
@@ -5250,7 +5250,7 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E182">
@@ -5276,7 +5276,7 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E183">
@@ -5302,7 +5302,7 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E184">
@@ -5328,7 +5328,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E185">
@@ -5380,7 +5380,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E187">
@@ -5406,7 +5406,7 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E188">
@@ -5458,7 +5458,7 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E190">
@@ -5484,7 +5484,7 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E191">
@@ -5562,7 +5562,7 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E194">
@@ -5588,7 +5588,7 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E195">
@@ -5614,7 +5614,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E196">
@@ -5666,7 +5666,7 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E198">
@@ -5718,7 +5718,7 @@
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E200">
@@ -5744,7 +5744,7 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E201">
@@ -5770,7 +5770,7 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E202">
@@ -5822,7 +5822,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E204">
@@ -5926,7 +5926,7 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E208">
@@ -5952,7 +5952,7 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E209">
@@ -5978,7 +5978,7 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E210">
@@ -6004,7 +6004,7 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E211">
@@ -6030,7 +6030,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E212">
@@ -6056,7 +6056,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E213">
@@ -6108,7 +6108,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E215">
@@ -6134,7 +6134,7 @@
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E216">
@@ -6212,7 +6212,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E219">
@@ -6264,7 +6264,7 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E221">
@@ -6316,7 +6316,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E223">
@@ -6342,7 +6342,7 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E224">
@@ -6394,7 +6394,7 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E226">
@@ -6420,7 +6420,7 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E227">
@@ -6446,7 +6446,7 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E228">
@@ -6472,7 +6472,7 @@
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E229">
@@ -6524,7 +6524,7 @@
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E231">
@@ -6550,7 +6550,7 @@
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E232">
@@ -6576,7 +6576,7 @@
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E233">
@@ -6602,7 +6602,7 @@
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E234">
@@ -6654,7 +6654,7 @@
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E236">
@@ -6680,7 +6680,7 @@
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E237">
@@ -6706,7 +6706,7 @@
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E238">
@@ -6732,7 +6732,7 @@
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E239">
@@ -6784,7 +6784,7 @@
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E241">
@@ -6810,7 +6810,7 @@
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E242">
@@ -6836,7 +6836,7 @@
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E243">
@@ -6888,7 +6888,7 @@
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E245">
@@ -6914,7 +6914,7 @@
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E246">
@@ -6966,7 +6966,7 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E248">
@@ -6992,7 +6992,7 @@
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E249">
@@ -7018,7 +7018,7 @@
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E250">
@@ -7096,7 +7096,7 @@
       </c>
       <c r="D253" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E253">
@@ -7122,7 +7122,7 @@
       </c>
       <c r="D254" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E254">
@@ -7148,7 +7148,7 @@
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E255">
@@ -7200,7 +7200,7 @@
       </c>
       <c r="D257" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E257">
@@ -7226,7 +7226,7 @@
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E258">
@@ -7252,7 +7252,7 @@
       </c>
       <c r="D259" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E259">
@@ -7330,7 +7330,7 @@
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E262">
@@ -7382,7 +7382,7 @@
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E264">
@@ -7434,7 +7434,7 @@
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E266">
@@ -7460,7 +7460,7 @@
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E267">
@@ -7512,7 +7512,7 @@
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E269">
@@ -7590,7 +7590,7 @@
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E272">
@@ -7642,7 +7642,7 @@
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E274">
@@ -7668,7 +7668,7 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E275">
@@ -7720,7 +7720,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E277">
@@ -7772,7 +7772,7 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E279">
@@ -7798,7 +7798,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E280">
@@ -7824,7 +7824,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E281">
@@ -7850,7 +7850,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E282">
@@ -7876,7 +7876,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E283">
@@ -7902,7 +7902,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E284">
@@ -7954,7 +7954,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E286">
@@ -7980,7 +7980,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E287">
@@ -8006,7 +8006,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E288">
@@ -8032,7 +8032,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E289">
@@ -8058,7 +8058,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E290">
@@ -8084,7 +8084,7 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E291">
@@ -8110,7 +8110,7 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E292">
@@ -8136,7 +8136,7 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E293">
@@ -8188,7 +8188,7 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E295">
@@ -8214,7 +8214,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E296">
@@ -8240,7 +8240,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E297">
@@ -8344,7 +8344,7 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E301">
@@ -8370,7 +8370,7 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E302">
@@ -8396,7 +8396,7 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E303">
@@ -8474,7 +8474,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E306">
@@ -8552,7 +8552,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E309">
@@ -8604,7 +8604,7 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E311">
@@ -8656,7 +8656,7 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E313">
@@ -8682,7 +8682,7 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E314">
@@ -8708,7 +8708,7 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E315">
@@ -8734,7 +8734,7 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E316">
@@ -8786,7 +8786,7 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E318">
@@ -8812,7 +8812,7 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E319">
@@ -8864,7 +8864,7 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E321">
@@ -8890,7 +8890,7 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E322">
@@ -8916,7 +8916,7 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E323">
@@ -8942,7 +8942,7 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E324">
@@ -8994,7 +8994,7 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E326">
@@ -9046,7 +9046,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E328">
@@ -9072,7 +9072,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E329">
@@ -9098,7 +9098,7 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E330">
@@ -9150,7 +9150,7 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E332">
@@ -9176,7 +9176,7 @@
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E333">
@@ -9202,7 +9202,7 @@
       </c>
       <c r="D334" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E334">
@@ -9228,7 +9228,7 @@
       </c>
       <c r="D335" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E335">
@@ -9254,7 +9254,7 @@
       </c>
       <c r="D336" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E336">
@@ -9280,7 +9280,7 @@
       </c>
       <c r="D337" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E337">
@@ -9306,7 +9306,7 @@
       </c>
       <c r="D338" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E338">
@@ -9358,7 +9358,7 @@
       </c>
       <c r="D340" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E340">
@@ -9384,7 +9384,7 @@
       </c>
       <c r="D341" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E341">
@@ -9410,7 +9410,7 @@
       </c>
       <c r="D342" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E342">
@@ -9436,7 +9436,7 @@
       </c>
       <c r="D343" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E343">
@@ -9462,7 +9462,7 @@
       </c>
       <c r="D344" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E344">
@@ -9488,7 +9488,7 @@
       </c>
       <c r="D345" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E345">
@@ -9566,7 +9566,7 @@
       </c>
       <c r="D348" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E348">
@@ -9592,7 +9592,7 @@
       </c>
       <c r="D349" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E349">
@@ -9618,7 +9618,7 @@
       </c>
       <c r="D350" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E350">
@@ -9670,7 +9670,7 @@
       </c>
       <c r="D352" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E352">
@@ -9722,7 +9722,7 @@
       </c>
       <c r="D354" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E354">
@@ -9800,7 +9800,7 @@
       </c>
       <c r="D357" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E357">
@@ -9878,7 +9878,7 @@
       </c>
       <c r="D360" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E360">
@@ -9930,7 +9930,7 @@
       </c>
       <c r="D362" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E362">
@@ -9956,7 +9956,7 @@
       </c>
       <c r="D363" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E363">
@@ -10034,7 +10034,7 @@
       </c>
       <c r="D366" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E366">
@@ -10060,7 +10060,7 @@
       </c>
       <c r="D367" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E367">
@@ -10086,7 +10086,7 @@
       </c>
       <c r="D368" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E368">
@@ -10112,7 +10112,7 @@
       </c>
       <c r="D369" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E369">
@@ -10138,7 +10138,7 @@
       </c>
       <c r="D370" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E370">
@@ -10164,7 +10164,7 @@
       </c>
       <c r="D371" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E371">
@@ -10190,7 +10190,7 @@
       </c>
       <c r="D372" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E372">
@@ -10268,7 +10268,7 @@
       </c>
       <c r="D375" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E375">
@@ -10320,7 +10320,7 @@
       </c>
       <c r="D377" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E377">
@@ -10372,7 +10372,7 @@
       </c>
       <c r="D379" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E379">
@@ -10450,7 +10450,7 @@
       </c>
       <c r="D382" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E382">
@@ -10502,7 +10502,7 @@
       </c>
       <c r="D384" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E384">
@@ -10528,7 +10528,7 @@
       </c>
       <c r="D385" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E385">
@@ -11133,19 +11133,19 @@
         </is>
       </c>
       <c r="B8" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.5, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="C8" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;4.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="D8" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;2.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="E8" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
     </row>
@@ -11156,19 +11156,19 @@
         </is>
       </c>
       <c r="B9" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.5, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="C9" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;4.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="D9" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;2.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="E9" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
     </row>
@@ -11179,19 +11179,19 @@
         </is>
       </c>
       <c r="B10" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.5, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="C10" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;4.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="D10" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;2.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="E10" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
     </row>
@@ -11202,19 +11202,19 @@
         </is>
       </c>
       <c r="B11" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.5, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="C11" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;4.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="D11" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;2.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="E11" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
     </row>
@@ -11225,19 +11225,19 @@
         </is>
       </c>
       <c r="B12" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.5, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="C12" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;4.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="D12" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;2.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="E12" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
     </row>
@@ -11248,19 +11248,19 @@
         </is>
       </c>
       <c r="B13" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.5, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="C13" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;4.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="D13" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;2.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="E13" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
     </row>
@@ -11271,19 +11271,19 @@
         </is>
       </c>
       <c r="B14" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.5, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="C14" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;4.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="D14" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;2.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
       <c r="E14" s="6">
-        <f>IF(OR(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5), "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability"), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix Product Dashboard logic with correct availability rules
New Product Availability Rules (in priority order):

1. Full Support (In-Region)
   - 100% of dependencies are GA in selected region

2. Full Support (Cross-Region)
   - 100% of dependencies are GA in at least one region

3. Limited Availability
   - Availability >= 70% and < 100%
   - Available = GA locally OR LA locally OR GA cross-region

4. Not Supported
   - Availability < 70%

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Product Language Matrix/Smart_Availability_Matrix.xlsx
+++ b/Product Language Matrix/Smart_Availability_Matrix.xlsx
@@ -596,7 +596,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E3">
@@ -622,7 +622,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E4">
@@ -648,7 +648,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E5">
@@ -674,7 +674,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E6">
@@ -700,7 +700,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E7">
@@ -726,7 +726,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E8">
@@ -752,7 +752,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E9">
@@ -804,7 +804,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E11">
@@ -882,7 +882,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E14">
@@ -960,7 +960,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E17">
@@ -1090,7 +1090,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E22">
@@ -1116,7 +1116,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E23">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E25">
@@ -1194,7 +1194,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E26">
@@ -1220,7 +1220,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E27">
@@ -1246,7 +1246,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E28">
@@ -1272,7 +1272,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E29">
@@ -1298,7 +1298,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E30">
@@ -1324,7 +1324,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E31">
@@ -1376,7 +1376,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E33">
@@ -1402,7 +1402,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E34">
@@ -1454,7 +1454,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E36">
@@ -1532,7 +1532,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E39">
@@ -1584,7 +1584,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E41">
@@ -1636,7 +1636,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E43">
@@ -1662,7 +1662,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E44">
@@ -1740,7 +1740,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E47">
@@ -1792,7 +1792,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E49">
@@ -1818,7 +1818,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E50">
@@ -1870,7 +1870,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E52">
@@ -1896,7 +1896,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E53">
@@ -1922,7 +1922,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E54">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E55">
@@ -2000,7 +2000,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E57">
@@ -2078,7 +2078,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E60">
@@ -2104,7 +2104,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E61">
@@ -2156,7 +2156,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E63">
@@ -2182,7 +2182,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E64">
@@ -2234,7 +2234,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E66">
@@ -2338,7 +2338,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E70">
@@ -2364,7 +2364,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E71">
@@ -2390,7 +2390,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E72">
@@ -2520,7 +2520,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E77">
@@ -2676,7 +2676,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E83">
@@ -2754,7 +2754,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E86">
@@ -2780,7 +2780,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E87">
@@ -2832,7 +2832,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E89">
@@ -2858,7 +2858,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E90">
@@ -2884,7 +2884,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E91">
@@ -2910,7 +2910,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E92">
@@ -2962,7 +2962,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E94">
@@ -2988,7 +2988,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E95">
@@ -3040,7 +3040,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E97">
@@ -3066,7 +3066,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E98">
@@ -3092,7 +3092,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E99">
@@ -3118,7 +3118,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E100">
@@ -3196,7 +3196,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E103">
@@ -3248,7 +3248,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E105">
@@ -3274,7 +3274,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E106">
@@ -3300,7 +3300,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E107">
@@ -3326,7 +3326,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E108">
@@ -3352,7 +3352,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E109">
@@ -3378,7 +3378,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E110">
@@ -3404,7 +3404,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E111">
@@ -3430,7 +3430,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E112">
@@ -3456,7 +3456,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E113">
@@ -3482,7 +3482,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E114">
@@ -3508,7 +3508,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E115">
@@ -3534,7 +3534,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E116">
@@ -3586,7 +3586,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E118">
@@ -3638,7 +3638,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E120">
@@ -3690,7 +3690,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E122">
@@ -3716,7 +3716,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E123">
@@ -3768,7 +3768,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E125">
@@ -3794,7 +3794,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E126">
@@ -3820,7 +3820,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E127">
@@ -3846,7 +3846,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E128">
@@ -3872,7 +3872,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E129">
@@ -3898,7 +3898,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E130">
@@ -3924,7 +3924,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E131">
@@ -3950,7 +3950,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E132">
@@ -3976,7 +3976,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E133">
@@ -4002,7 +4002,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E134">
@@ -4028,7 +4028,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E135">
@@ -4054,7 +4054,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E136">
@@ -4080,7 +4080,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E137">
@@ -4106,7 +4106,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E138">
@@ -4132,7 +4132,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E139">
@@ -4184,7 +4184,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E141">
@@ -4210,7 +4210,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E142">
@@ -4262,7 +4262,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E144">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E145">
@@ -4314,7 +4314,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E146">
@@ -4340,7 +4340,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E147">
@@ -4366,7 +4366,7 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E148">
@@ -4418,7 +4418,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E150">
@@ -4496,7 +4496,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E153">
@@ -4548,7 +4548,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E155">
@@ -4574,7 +4574,7 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E156">
@@ -4600,7 +4600,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E157">
@@ -4626,7 +4626,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E158">
@@ -4652,7 +4652,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E159">
@@ -4678,7 +4678,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E160">
@@ -4704,7 +4704,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E161">
@@ -4730,7 +4730,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E162">
@@ -4782,7 +4782,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E164">
@@ -4834,7 +4834,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E166">
@@ -4860,7 +4860,7 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E167">
@@ -4886,7 +4886,7 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E168">
@@ -4912,7 +4912,7 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E169">
@@ -4964,7 +4964,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E171">
@@ -4990,7 +4990,7 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E172">
@@ -5016,7 +5016,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E173">
@@ -5042,7 +5042,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E174">
@@ -5068,7 +5068,7 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E175">
@@ -5146,7 +5146,7 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E178">
@@ -5172,7 +5172,7 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E179">
@@ -5198,7 +5198,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E180">
@@ -5224,7 +5224,7 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E181">
@@ -5250,7 +5250,7 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E182">
@@ -5276,7 +5276,7 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E183">
@@ -5302,7 +5302,7 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E184">
@@ -5328,7 +5328,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E185">
@@ -5484,7 +5484,7 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E191">
@@ -5536,7 +5536,7 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E193">
@@ -5562,7 +5562,7 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E194">
@@ -5666,7 +5666,7 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E198">
@@ -5718,7 +5718,7 @@
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E200">
@@ -5796,7 +5796,7 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E203">
@@ -5822,7 +5822,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E204">
@@ -5848,7 +5848,7 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E205">
@@ -5874,7 +5874,7 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E206">
@@ -5900,7 +5900,7 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E207">
@@ -5926,7 +5926,7 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E208">
@@ -6004,7 +6004,7 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E211">
@@ -6030,7 +6030,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E212">
@@ -6082,7 +6082,7 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E214">
@@ -6108,7 +6108,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E215">
@@ -6134,7 +6134,7 @@
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E216">
@@ -6160,7 +6160,7 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E217">
@@ -6212,7 +6212,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E219">
@@ -6238,7 +6238,7 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E220">
@@ -6290,7 +6290,7 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E222">
@@ -6316,7 +6316,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E223">
@@ -6342,7 +6342,7 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E224">
@@ -6394,7 +6394,7 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E226">
@@ -6420,7 +6420,7 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E227">
@@ -6446,7 +6446,7 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E228">
@@ -6472,7 +6472,7 @@
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E229">
@@ -6498,7 +6498,7 @@
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E230">
@@ -6550,7 +6550,7 @@
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E232">
@@ -6576,7 +6576,7 @@
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E233">
@@ -6628,7 +6628,7 @@
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E235">
@@ -6654,7 +6654,7 @@
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E236">
@@ -6680,7 +6680,7 @@
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E237">
@@ -6706,7 +6706,7 @@
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E238">
@@ -6784,7 +6784,7 @@
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E241">
@@ -6810,7 +6810,7 @@
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E242">
@@ -6940,7 +6940,7 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E247">
@@ -7018,7 +7018,7 @@
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E250">
@@ -7096,7 +7096,7 @@
       </c>
       <c r="D253" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E253">
@@ -7122,7 +7122,7 @@
       </c>
       <c r="D254" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E254">
@@ -7148,7 +7148,7 @@
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E255">
@@ -7200,7 +7200,7 @@
       </c>
       <c r="D257" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E257">
@@ -7226,7 +7226,7 @@
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E258">
@@ -7304,7 +7304,7 @@
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E261">
@@ -7356,7 +7356,7 @@
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E263">
@@ -7382,7 +7382,7 @@
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E264">
@@ -7434,7 +7434,7 @@
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E266">
@@ -7460,7 +7460,7 @@
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E267">
@@ -7486,7 +7486,7 @@
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E268">
@@ -7538,7 +7538,7 @@
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E270">
@@ -7616,7 +7616,7 @@
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E273">
@@ -7642,7 +7642,7 @@
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E274">
@@ -7668,7 +7668,7 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E275">
@@ -7720,7 +7720,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E277">
@@ -7772,7 +7772,7 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E279">
@@ -7798,7 +7798,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E280">
@@ -7824,7 +7824,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E281">
@@ -7850,7 +7850,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E282">
@@ -7902,7 +7902,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E284">
@@ -7980,7 +7980,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E287">
@@ -8006,7 +8006,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E288">
@@ -8162,7 +8162,7 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E294">
@@ -8188,7 +8188,7 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E295">
@@ -8240,7 +8240,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E297">
@@ -8266,7 +8266,7 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E298">
@@ -8292,7 +8292,7 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E299">
@@ -8318,7 +8318,7 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E300">
@@ -8422,7 +8422,7 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E304">
@@ -8448,7 +8448,7 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E305">
@@ -8474,7 +8474,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E306">
@@ -8552,7 +8552,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E309">
@@ -8578,7 +8578,7 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E310">
@@ -8604,7 +8604,7 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E311">
@@ -8630,7 +8630,7 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E312">
@@ -8656,7 +8656,7 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E313">
@@ -8812,7 +8812,7 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E319">
@@ -8890,7 +8890,7 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E322">
@@ -8916,7 +8916,7 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E323">
@@ -8942,7 +8942,7 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E324">
@@ -9020,7 +9020,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E327">
@@ -9046,7 +9046,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E328">
@@ -9098,7 +9098,7 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E330">
@@ -9124,7 +9124,7 @@
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E331">
@@ -9176,7 +9176,7 @@
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E333">
@@ -9228,7 +9228,7 @@
       </c>
       <c r="D335" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E335">
@@ -9332,7 +9332,7 @@
       </c>
       <c r="D339" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E339">
@@ -9358,7 +9358,7 @@
       </c>
       <c r="D340" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E340">
@@ -9384,7 +9384,7 @@
       </c>
       <c r="D341" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E341">
@@ -9410,7 +9410,7 @@
       </c>
       <c r="D342" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E342">
@@ -9436,7 +9436,7 @@
       </c>
       <c r="D343" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E343">
@@ -9488,7 +9488,7 @@
       </c>
       <c r="D345" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E345">
@@ -9540,7 +9540,7 @@
       </c>
       <c r="D347" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E347">
@@ -9566,7 +9566,7 @@
       </c>
       <c r="D348" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E348">
@@ -9592,7 +9592,7 @@
       </c>
       <c r="D349" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E349">
@@ -9644,7 +9644,7 @@
       </c>
       <c r="D351" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E351">
@@ -9748,7 +9748,7 @@
       </c>
       <c r="D355" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E355">
@@ -9774,7 +9774,7 @@
       </c>
       <c r="D356" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E356">
@@ -9826,7 +9826,7 @@
       </c>
       <c r="D358" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E358">
@@ -9852,7 +9852,7 @@
       </c>
       <c r="D359" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E359">
@@ -9878,7 +9878,7 @@
       </c>
       <c r="D360" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E360">
@@ -9904,7 +9904,7 @@
       </c>
       <c r="D361" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E361">
@@ -9930,7 +9930,7 @@
       </c>
       <c r="D362" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E362">
@@ -9982,7 +9982,7 @@
       </c>
       <c r="D364" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E364">
@@ -10008,7 +10008,7 @@
       </c>
       <c r="D365" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E365">
@@ -10060,7 +10060,7 @@
       </c>
       <c r="D367" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E367">
@@ -10138,7 +10138,7 @@
       </c>
       <c r="D370" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E370">
@@ -10216,7 +10216,7 @@
       </c>
       <c r="D373" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E373">
@@ -10268,7 +10268,7 @@
       </c>
       <c r="D375" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E375">
@@ -10294,7 +10294,7 @@
       </c>
       <c r="D376" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E376">
@@ -10320,7 +10320,7 @@
       </c>
       <c r="D377" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E377">
@@ -10346,7 +10346,7 @@
       </c>
       <c r="D378" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E378">
@@ -10398,7 +10398,7 @@
       </c>
       <c r="D380" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E380">
@@ -10450,7 +10450,7 @@
       </c>
       <c r="D382" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E382">
@@ -10502,7 +10502,7 @@
       </c>
       <c r="D384" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E384">
@@ -10528,7 +10528,7 @@
       </c>
       <c r="D385" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E385">
@@ -11133,19 +11133,19 @@
         </is>
       </c>
       <c r="B8" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.5, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0))=3, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=3, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/3)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="C8" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;4.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0))=8, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=8, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/8)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="D8" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;2.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0))=4, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=4, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/4)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="E8" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0))=2, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=2, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/2)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
     </row>
@@ -11156,19 +11156,19 @@
         </is>
       </c>
       <c r="B9" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.5, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0))=3, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=3, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/3)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="C9" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;4.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0))=8, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=8, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/8)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="D9" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;2.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0))=4, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=4, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/4)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="E9" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0))=2, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=2, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/2)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
     </row>
@@ -11179,19 +11179,19 @@
         </is>
       </c>
       <c r="B10" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.5, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0))=3, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=3, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/3)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="C10" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;4.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0))=8, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=8, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/8)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="D10" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;2.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0))=4, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=4, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/4)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="E10" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0))=2, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=2, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/2)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
     </row>
@@ -11202,19 +11202,19 @@
         </is>
       </c>
       <c r="B11" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.5, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0))=3, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=3, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/3)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="C11" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;4.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0))=8, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=8, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/8)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="D11" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;2.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0))=4, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=4, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/4)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="E11" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0))=2, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=2, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/2)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
     </row>
@@ -11225,19 +11225,19 @@
         </is>
       </c>
       <c r="B12" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.5, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0))=3, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=3, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/3)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="C12" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;4.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0))=8, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=8, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/8)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="D12" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;2.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0))=4, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=4, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/4)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="E12" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0))=2, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=2, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/2)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
     </row>
@@ -11248,19 +11248,19 @@
         </is>
       </c>
       <c r="B13" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.5, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0))=3, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=3, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/3)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="C13" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;4.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0))=8, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=8, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/8)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="D13" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;2.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0))=4, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=4, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/4)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="E13" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0))=2, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=2, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/2)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
     </row>
@@ -11271,19 +11271,19 @@
         </is>
       </c>
       <c r="B14" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.5, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0))=3, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=3, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/3)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="C14" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;4.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0))=8, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=8, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/8)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="D14" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;2.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0))=4, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=4, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/4)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="E14" s="6">
-        <f>IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,1,0))&gt;1.0, "Not Supported", IF(OR(AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5),AND(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Not Supported", COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")&lt;5)), "Full Support (Cross-Region)", IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5,COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"Not Supported")=5), "Limited Availability", "Full Support (In-Region)")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0))=2, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=2, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/2)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Change Limited Availability threshold from 70% to 50%
Product is now Limited Availability if >= 50% of dependencies
are available (GA locally, LA locally, or GA cross-region).

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Product Language Matrix/Smart_Availability_Matrix.xlsx
+++ b/Product Language Matrix/Smart_Availability_Matrix.xlsx
@@ -570,7 +570,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E2">
@@ -622,7 +622,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E4">
@@ -648,7 +648,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E5">
@@ -726,7 +726,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E8">
@@ -830,7 +830,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E12">
@@ -856,7 +856,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E13">
@@ -908,7 +908,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E15">
@@ -960,7 +960,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E17">
@@ -986,7 +986,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E18">
@@ -1038,7 +1038,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E20">
@@ -1064,7 +1064,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E21">
@@ -1090,7 +1090,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E22">
@@ -1116,7 +1116,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E23">
@@ -1194,7 +1194,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E26">
@@ -1220,7 +1220,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E27">
@@ -1298,7 +1298,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E30">
@@ -1324,7 +1324,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E31">
@@ -1376,7 +1376,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E33">
@@ -1402,7 +1402,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E34">
@@ -1428,7 +1428,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E35">
@@ -1454,7 +1454,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E36">
@@ -1480,7 +1480,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E37">
@@ -1506,7 +1506,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E38">
@@ -1532,7 +1532,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E39">
@@ -1558,7 +1558,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E40">
@@ -1584,7 +1584,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E41">
@@ -1662,7 +1662,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E44">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E45">
@@ -1740,7 +1740,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E47">
@@ -1766,7 +1766,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E48">
@@ -1792,7 +1792,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E49">
@@ -1818,7 +1818,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E50">
@@ -1844,7 +1844,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E51">
@@ -1870,7 +1870,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E52">
@@ -1896,7 +1896,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E53">
@@ -1922,7 +1922,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E54">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E55">
@@ -2000,7 +2000,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E57">
@@ -2026,7 +2026,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E58">
@@ -2052,7 +2052,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E59">
@@ -2078,7 +2078,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E60">
@@ -2130,7 +2130,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E62">
@@ -2156,7 +2156,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E63">
@@ -2182,7 +2182,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E64">
@@ -2234,7 +2234,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E66">
@@ -2286,7 +2286,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E68">
@@ -2312,7 +2312,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E69">
@@ -2338,7 +2338,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E70">
@@ -2416,7 +2416,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E73">
@@ -2442,7 +2442,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E74">
@@ -2468,7 +2468,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E75">
@@ -2520,7 +2520,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E77">
@@ -2546,7 +2546,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E78">
@@ -2598,7 +2598,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E80">
@@ -2650,7 +2650,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E82">
@@ -2676,7 +2676,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E83">
@@ -2702,7 +2702,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E84">
@@ -2728,7 +2728,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E85">
@@ -2754,7 +2754,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E86">
@@ -2780,7 +2780,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E87">
@@ -2910,7 +2910,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E92">
@@ -2936,7 +2936,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E93">
@@ -2988,7 +2988,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E95">
@@ -3040,7 +3040,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E97">
@@ -3066,7 +3066,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E98">
@@ -3118,7 +3118,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E100">
@@ -3144,7 +3144,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E101">
@@ -3170,7 +3170,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E102">
@@ -3196,7 +3196,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E103">
@@ -3222,7 +3222,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E104">
@@ -3274,7 +3274,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E106">
@@ -3300,7 +3300,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E107">
@@ -3326,7 +3326,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E108">
@@ -3404,7 +3404,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E111">
@@ -3430,7 +3430,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E112">
@@ -3482,7 +3482,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E114">
@@ -3508,7 +3508,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E115">
@@ -3534,7 +3534,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E116">
@@ -3560,7 +3560,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E117">
@@ -3586,7 +3586,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E118">
@@ -3690,7 +3690,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E122">
@@ -3716,7 +3716,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E123">
@@ -3768,7 +3768,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E125">
@@ -3794,7 +3794,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E126">
@@ -3820,7 +3820,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E127">
@@ -3846,7 +3846,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E128">
@@ -3924,7 +3924,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E131">
@@ -3976,7 +3976,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E133">
@@ -4106,7 +4106,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E138">
@@ -4132,7 +4132,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E139">
@@ -4158,7 +4158,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E140">
@@ -4184,7 +4184,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E141">
@@ -4314,7 +4314,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E146">
@@ -4340,7 +4340,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E147">
@@ -4392,7 +4392,7 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E149">
@@ -4418,7 +4418,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E150">
@@ -4444,7 +4444,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E151">
@@ -4470,7 +4470,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E152">
@@ -4496,7 +4496,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E153">
@@ -4522,7 +4522,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E154">
@@ -4548,7 +4548,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E155">
@@ -4574,7 +4574,7 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E156">
@@ -4600,7 +4600,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E157">
@@ -4626,7 +4626,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E158">
@@ -4678,7 +4678,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E160">
@@ -4704,7 +4704,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E161">
@@ -4730,7 +4730,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E162">
@@ -4756,7 +4756,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E163">
@@ -4782,7 +4782,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E164">
@@ -4834,7 +4834,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E166">
@@ -4912,7 +4912,7 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E169">
@@ -4964,7 +4964,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E171">
@@ -4990,7 +4990,7 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E172">
@@ -5016,7 +5016,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E173">
@@ -5042,7 +5042,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E174">
@@ -5094,7 +5094,7 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E176">
@@ -5146,7 +5146,7 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E178">
@@ -5198,7 +5198,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E180">
@@ -5224,7 +5224,7 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E181">
@@ -5276,7 +5276,7 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E183">
@@ -5302,7 +5302,7 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E184">
@@ -5328,7 +5328,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E185">
@@ -5354,7 +5354,7 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E186">
@@ -5380,7 +5380,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E187">
@@ -5406,7 +5406,7 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E188">
@@ -5484,7 +5484,7 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E191">
@@ -5510,7 +5510,7 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E192">
@@ -5614,7 +5614,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E196">
@@ -5692,7 +5692,7 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E199">
@@ -5718,7 +5718,7 @@
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E200">
@@ -5744,7 +5744,7 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E201">
@@ -5770,7 +5770,7 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E202">
@@ -5796,7 +5796,7 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E203">
@@ -5822,7 +5822,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E204">
@@ -5874,7 +5874,7 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E206">
@@ -5900,7 +5900,7 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E207">
@@ -5952,7 +5952,7 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E209">
@@ -5978,7 +5978,7 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E210">
@@ -6056,7 +6056,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E213">
@@ -6082,7 +6082,7 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E214">
@@ -6108,7 +6108,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E215">
@@ -6212,7 +6212,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E219">
@@ -6264,7 +6264,7 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E221">
@@ -6290,7 +6290,7 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E222">
@@ -6316,7 +6316,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E223">
@@ -6342,7 +6342,7 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E224">
@@ -6368,7 +6368,7 @@
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E225">
@@ -6446,7 +6446,7 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E228">
@@ -6472,7 +6472,7 @@
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E229">
@@ -6550,7 +6550,7 @@
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E232">
@@ -6576,7 +6576,7 @@
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E233">
@@ -6602,7 +6602,7 @@
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E234">
@@ -6628,7 +6628,7 @@
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E235">
@@ -6706,7 +6706,7 @@
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E238">
@@ -6758,7 +6758,7 @@
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E240">
@@ -6810,7 +6810,7 @@
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E242">
@@ -6914,7 +6914,7 @@
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E246">
@@ -6940,7 +6940,7 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E247">
@@ -6966,7 +6966,7 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E248">
@@ -7018,7 +7018,7 @@
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E250">
@@ -7044,7 +7044,7 @@
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E251">
@@ -7122,7 +7122,7 @@
       </c>
       <c r="D254" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E254">
@@ -7226,7 +7226,7 @@
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E258">
@@ -7304,7 +7304,7 @@
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E261">
@@ -7434,7 +7434,7 @@
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E266">
@@ -7460,7 +7460,7 @@
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E267">
@@ -7512,7 +7512,7 @@
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E269">
@@ -7538,7 +7538,7 @@
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E270">
@@ -7564,7 +7564,7 @@
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E271">
@@ -7642,7 +7642,7 @@
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E274">
@@ -7668,7 +7668,7 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E275">
@@ -7694,7 +7694,7 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E276">
@@ -7746,7 +7746,7 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E278">
@@ -7798,7 +7798,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E280">
@@ -7824,7 +7824,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E281">
@@ -7876,7 +7876,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E283">
@@ -7902,7 +7902,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E284">
@@ -7928,7 +7928,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E285">
@@ -7954,7 +7954,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E286">
@@ -8006,7 +8006,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E288">
@@ -8058,7 +8058,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E290">
@@ -8110,7 +8110,7 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E292">
@@ -8162,7 +8162,7 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E294">
@@ -8188,7 +8188,7 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E295">
@@ -8214,7 +8214,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E296">
@@ -8240,7 +8240,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E297">
@@ -8292,7 +8292,7 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E299">
@@ -8370,7 +8370,7 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E302">
@@ -8396,7 +8396,7 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E303">
@@ -8422,7 +8422,7 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E304">
@@ -8448,7 +8448,7 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E305">
@@ -8474,7 +8474,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E306">
@@ -8578,7 +8578,7 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E310">
@@ -8604,7 +8604,7 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E311">
@@ -8630,7 +8630,7 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E312">
@@ -8734,7 +8734,7 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E316">
@@ -8760,7 +8760,7 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E317">
@@ -8786,7 +8786,7 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E318">
@@ -8812,7 +8812,7 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E319">
@@ -8838,7 +8838,7 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E320">
@@ -8916,7 +8916,7 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E323">
@@ -8942,7 +8942,7 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E324">
@@ -8994,7 +8994,7 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E326">
@@ -9020,7 +9020,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E327">
@@ -9072,7 +9072,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E329">
@@ -9098,7 +9098,7 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E330">
@@ -9124,7 +9124,7 @@
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E331">
@@ -9150,7 +9150,7 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E332">
@@ -9176,7 +9176,7 @@
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E333">
@@ -9202,7 +9202,7 @@
       </c>
       <c r="D334" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E334">
@@ -9254,7 +9254,7 @@
       </c>
       <c r="D336" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E336">
@@ -9306,7 +9306,7 @@
       </c>
       <c r="D338" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E338">
@@ -9332,7 +9332,7 @@
       </c>
       <c r="D339" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E339">
@@ -9384,7 +9384,7 @@
       </c>
       <c r="D341" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E341">
@@ -9436,7 +9436,7 @@
       </c>
       <c r="D343" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E343">
@@ -9592,7 +9592,7 @@
       </c>
       <c r="D349" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E349">
@@ -9670,7 +9670,7 @@
       </c>
       <c r="D352" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E352">
@@ -9696,7 +9696,7 @@
       </c>
       <c r="D353" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E353">
@@ -9722,7 +9722,7 @@
       </c>
       <c r="D354" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E354">
@@ -9748,7 +9748,7 @@
       </c>
       <c r="D355" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E355">
@@ -9774,7 +9774,7 @@
       </c>
       <c r="D356" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E356">
@@ -9826,7 +9826,7 @@
       </c>
       <c r="D358" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E358">
@@ -9852,7 +9852,7 @@
       </c>
       <c r="D359" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E359">
@@ -9878,7 +9878,7 @@
       </c>
       <c r="D360" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E360">
@@ -9956,7 +9956,7 @@
       </c>
       <c r="D363" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E363">
@@ -9982,7 +9982,7 @@
       </c>
       <c r="D364" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E364">
@@ -10008,7 +10008,7 @@
       </c>
       <c r="D365" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E365">
@@ -10034,7 +10034,7 @@
       </c>
       <c r="D366" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E366">
@@ -10060,7 +10060,7 @@
       </c>
       <c r="D367" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E367">
@@ -10086,7 +10086,7 @@
       </c>
       <c r="D368" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E368">
@@ -10112,7 +10112,7 @@
       </c>
       <c r="D369" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E369">
@@ -10138,7 +10138,7 @@
       </c>
       <c r="D370" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E370">
@@ -10190,7 +10190,7 @@
       </c>
       <c r="D372" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E372">
@@ -10216,7 +10216,7 @@
       </c>
       <c r="D373" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E373">
@@ -10242,7 +10242,7 @@
       </c>
       <c r="D374" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E374">
@@ -10268,7 +10268,7 @@
       </c>
       <c r="D375" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E375">
@@ -10294,7 +10294,7 @@
       </c>
       <c r="D376" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E376">
@@ -10320,7 +10320,7 @@
       </c>
       <c r="D377" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E377">
@@ -10346,7 +10346,7 @@
       </c>
       <c r="D378" t="inlineStr">
         <is>
-          <t>Not Supported</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E378">
@@ -10372,7 +10372,7 @@
       </c>
       <c r="D379" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>Not Supported</t>
         </is>
       </c>
       <c r="E379">
@@ -10476,7 +10476,7 @@
       </c>
       <c r="D383" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E383">
@@ -10528,7 +10528,7 @@
       </c>
       <c r="D385" t="inlineStr">
         <is>
-          <t>Limited Availability</t>
+          <t>General Availability</t>
         </is>
       </c>
       <c r="E385">
@@ -10554,7 +10554,7 @@
       </c>
       <c r="D386" t="inlineStr">
         <is>
-          <t>General Availability</t>
+          <t>Limited Availability</t>
         </is>
       </c>
       <c r="E386">
@@ -11133,19 +11133,19 @@
         </is>
       </c>
       <c r="B8" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0))=3, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=3, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/3)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0))=3, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=3, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/3)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="C8" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0))=8, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=8, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/8)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0))=8, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=8, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/8)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="D8" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0))=4, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=4, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/4)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0))=4, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=4, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/4)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="E8" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0))=2, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=2, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/2)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",1,0))=2, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=2, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A8, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A8,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/2)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
     </row>
@@ -11156,19 +11156,19 @@
         </is>
       </c>
       <c r="B9" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0))=3, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=3, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/3)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0))=3, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=3, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/3)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="C9" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0))=8, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=8, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/8)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0))=8, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=8, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/8)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="D9" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0))=4, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=4, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/4)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0))=4, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=4, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/4)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="E9" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0))=2, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=2, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/2)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",1,0))=2, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=2, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A9, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A9,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/2)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
     </row>
@@ -11179,19 +11179,19 @@
         </is>
       </c>
       <c r="B10" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0))=3, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=3, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/3)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0))=3, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=3, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/3)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="C10" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0))=8, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=8, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/8)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0))=8, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=8, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/8)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="D10" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0))=4, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=4, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/4)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0))=4, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=4, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/4)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="E10" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0))=2, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=2, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/2)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",1,0))=2, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=2, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A10, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A10,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/2)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
     </row>
@@ -11202,19 +11202,19 @@
         </is>
       </c>
       <c r="B11" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0))=3, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=3, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/3)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0))=3, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=3, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/3)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="C11" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0))=8, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=8, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/8)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0))=8, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=8, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/8)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="D11" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0))=4, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=4, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/4)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0))=4, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=4, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/4)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="E11" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0))=2, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=2, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/2)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",1,0))=2, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=2, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A11, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A11,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/2)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
     </row>
@@ -11225,19 +11225,19 @@
         </is>
       </c>
       <c r="B12" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0))=3, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=3, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/3)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0))=3, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=3, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/3)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="C12" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0))=8, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=8, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/8)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0))=8, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=8, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/8)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="D12" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0))=4, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=4, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/4)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0))=4, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=4, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/4)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="E12" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0))=2, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=2, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/2)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",1,0))=2, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=2, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A12, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A12,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/2)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
     </row>
@@ -11248,19 +11248,19 @@
         </is>
       </c>
       <c r="B13" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0))=3, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=3, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/3)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0))=3, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=3, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/3)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="C13" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0))=8, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=8, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/8)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0))=8, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=8, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/8)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="D13" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0))=4, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=4, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/4)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0))=4, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=4, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/4)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="E13" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0))=2, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=2, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/2)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",1,0))=2, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=2, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A13, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A13,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/2)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
     </row>
@@ -11271,19 +11271,19 @@
         </is>
       </c>
       <c r="B14" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0))=3, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=3, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/3)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0))=3, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=3, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|SSA-LLM|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"SSA-LLM",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/3)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="C14" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0))=8, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=8, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/8)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0))=8, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=8, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Intent (UniFit)|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Intent (UniFit)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Entity (NER/Spacy)|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Entity (NER/Spacy)",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Summary|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Summary",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|KaaS|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"KaaS",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Pro-active Service|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Pro-active Service",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/8)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="D14" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0))=4, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=4, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/4)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0))=4, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=4, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Gen AI Disposition|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Gen AI Disposition",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Conversation Facts|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Conversation Facts",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/4)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
       <c r="E14" s="6">
-        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0))=2, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=2, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/2)&gt;=0.7, "Limited Availability", "Not Supported")))</f>
+        <f>IF((IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0)+IF(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",1,0))=2, "Full Support (In-Region)", IF((IF(COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0)+IF(COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1,1,0))=2, "Full Support (Cross-Region)", IF(((IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|ASR|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"ASR",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0)+IF(OR(INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="General Availability",INDEX(Service_Input!$D:$D, MATCH($C$4&amp;"|Redaction|"&amp;$A14, Service_Input!$E:$E, 0))="Limited Availability",COUNTIFS(Service_Input!$B:$B,"Redaction",Service_Input!$C:$C,$A14,Service_Input!$D:$D,"General Availability")&gt;=1),1,0))/2)&gt;=0.5, "Limited Availability", "Not Supported")))</f>
         <v/>
       </c>
     </row>

</xml_diff>